<commit_message>
update bom and version
</commit_message>
<xml_diff>
--- a/crimps/bom/BOM.Guide.xlsx
+++ b/crimps/bom/BOM.Guide.xlsx
@@ -1,25 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karl/Workspace/KiCad/Crimps/crimps/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karl/Workspace/KiCad/Crimps/crimps/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2828A41-76A2-D746-9F49-ABAC296AE807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="500" windowWidth="19120" windowHeight="17500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="6240" yWindow="740" windowWidth="19120" windowHeight="17500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
     <sheet name="GUIDE" sheetId="2" r:id="rId2"/>
     <sheet name="Costing" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -595,9 +607,6 @@
     <t>incoming eBay 2022</t>
   </si>
   <si>
-    <t>PJ301 THONKICONN6</t>
-  </si>
-  <si>
     <t>OPA4171</t>
   </si>
   <si>
@@ -625,9 +634,6 @@
     <t>Cap_THT:D6.3mm_P2.50mm</t>
   </si>
   <si>
-    <t>Crimps v121 karltron.com December 2021 - Derived from Mutable Kinks v4.1 cc-by-sa</t>
-  </si>
-  <si>
     <t>power cable</t>
   </si>
   <si>
@@ -659,16 +665,32 @@
   </si>
   <si>
     <t>J112 and MMBF4392 work too</t>
+  </si>
+  <si>
+    <t>Crimps v122 karltron.com December 2021 - Derived from Mutable Kinks v4.1 cc-by-sa</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PJ301 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>THONKICONN</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -704,6 +726,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="3">
@@ -784,14 +811,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -808,6 +835,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1075,7 +1105,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G117"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="A84" workbookViewId="0">
@@ -2864,14 +2894,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2885,7 +2915,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2925,7 +2955,7 @@
         <v>166</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -3025,7 +3055,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>144</v>
@@ -3034,7 +3064,7 @@
         <v>166</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -3080,7 +3110,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>171</v>
@@ -3164,13 +3194,13 @@
         <v>66</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>189</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -3187,7 +3217,7 @@
         <v>59</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F17" s="5"/>
     </row>
@@ -3205,7 +3235,7 @@
         <v>63</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F18" s="5"/>
     </row>
@@ -3226,7 +3256,7 @@
         <v>185</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -3266,7 +3296,7 @@
         <v>174</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -3283,10 +3313,10 @@
         <v>18</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -3345,7 +3375,7 @@
       </c>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -3356,7 +3386,7 @@
         <v>155</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>188</v>
+        <v>209</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>184</v>
@@ -3371,7 +3401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
@@ -3400,13 +3430,13 @@
         <v>169</v>
       </c>
       <c r="G1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I1" t="s">
         <v>201</v>
-      </c>
-      <c r="H1" t="s">
-        <v>202</v>
-      </c>
-      <c r="I1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="48" x14ac:dyDescent="0.2">
@@ -3462,13 +3492,13 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K3" t="s">
+        <v>202</v>
+      </c>
+      <c r="L3" t="s">
         <v>204</v>
       </c>
-      <c r="L3" t="s">
-        <v>206</v>
-      </c>
       <c r="M3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="48" x14ac:dyDescent="0.2">
@@ -3601,7 +3631,7 @@
         <v>166</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H8" s="13">
         <v>0.01</v>
@@ -4087,12 +4117,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B27" s="12">
         <v>1</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H27" s="13">
         <v>1</v>
@@ -4102,9 +4132,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C28" s="9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>